<commit_message>
added script for updating R
</commit_message>
<xml_diff>
--- a/00_20231118_srlwq_huber_all_scales.xlsx
+++ b/00_20231118_srlwq_huber_all_scales.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\workpl_srl_thesis_phhd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3C7053-C5F0-4BB8-A097-EFE39B0D00CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E77F1E-2721-474A-BA36-139E040608EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="likert_verbal" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1262,16 +1262,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A4D2ADC-F973-4D84-86CE-84155CB928A0}">
   <dimension ref="A1:BW108"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>86</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -3541,7 +3541,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -3768,7 +3768,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -3995,7 +3995,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -4222,7 +4222,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -4449,7 +4449,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -4676,7 +4676,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -4903,7 +4903,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -5130,7 +5130,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -5357,7 +5357,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -5584,7 +5584,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -5811,7 +5811,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -6038,7 +6038,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -6265,7 +6265,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -6492,7 +6492,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -6719,7 +6719,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -6946,7 +6946,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -7173,7 +7173,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -7400,7 +7400,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -7627,7 +7627,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -7854,7 +7854,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>148</v>
       </c>
@@ -8081,7 +8081,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="31" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -8308,7 +8308,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -8535,7 +8535,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -8762,7 +8762,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -8989,7 +8989,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -9216,7 +9216,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -9443,7 +9443,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="37" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -9670,7 +9670,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>13</v>
       </c>
@@ -9897,7 +9897,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -10124,7 +10124,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>28</v>
       </c>
@@ -10351,7 +10351,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -10578,7 +10578,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -10805,7 +10805,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>32</v>
       </c>
@@ -11032,7 +11032,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>36</v>
       </c>
@@ -11259,7 +11259,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>36</v>
       </c>
@@ -11486,7 +11486,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>28</v>
       </c>
@@ -11713,7 +11713,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>36</v>
       </c>
@@ -11940,7 +11940,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>36</v>
       </c>
@@ -12167,7 +12167,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>28</v>
       </c>
@@ -12394,7 +12394,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>32</v>
       </c>
@@ -12621,7 +12621,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>13</v>
       </c>
@@ -12848,7 +12848,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>32</v>
       </c>
@@ -13075,7 +13075,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>36</v>
       </c>
@@ -13302,7 +13302,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>36</v>
       </c>
@@ -13529,7 +13529,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="55" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>36</v>
       </c>
@@ -13756,7 +13756,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>13</v>
       </c>
@@ -13983,7 +13983,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>28</v>
       </c>
@@ -14210,7 +14210,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>28</v>
       </c>
@@ -14437,7 +14437,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>28</v>
       </c>
@@ -14664,7 +14664,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>52</v>
       </c>
@@ -14891,7 +14891,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>32</v>
       </c>
@@ -15118,7 +15118,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="62" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>32</v>
       </c>
@@ -15345,7 +15345,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>13</v>
       </c>
@@ -15572,7 +15572,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="64" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>36</v>
       </c>
@@ -15799,7 +15799,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>36</v>
       </c>
@@ -16026,7 +16026,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>32</v>
       </c>
@@ -16253,7 +16253,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="67" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>13</v>
       </c>
@@ -16480,7 +16480,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>13</v>
       </c>
@@ -16707,7 +16707,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="69" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>36</v>
       </c>
@@ -16934,7 +16934,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>36</v>
       </c>
@@ -17161,7 +17161,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>13</v>
       </c>
@@ -17388,7 +17388,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="72" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>28</v>
       </c>
@@ -17615,7 +17615,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="73" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>52</v>
       </c>
@@ -17842,7 +17842,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="74" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>52</v>
       </c>
@@ -18069,7 +18069,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>28</v>
       </c>
@@ -18296,7 +18296,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>28</v>
       </c>
@@ -18523,7 +18523,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="77" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>36</v>
       </c>
@@ -18750,7 +18750,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="78" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>28</v>
       </c>
@@ -18977,7 +18977,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>36</v>
       </c>
@@ -19204,7 +19204,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="80" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>28</v>
       </c>
@@ -19431,7 +19431,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>13</v>
       </c>
@@ -19658,7 +19658,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="82" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>36</v>
       </c>
@@ -19885,7 +19885,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>32</v>
       </c>
@@ -20112,7 +20112,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>28</v>
       </c>
@@ -20339,7 +20339,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="85" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>28</v>
       </c>
@@ -20566,7 +20566,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>28</v>
       </c>
@@ -20793,7 +20793,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>13</v>
       </c>
@@ -21020,7 +21020,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>13</v>
       </c>
@@ -21247,7 +21247,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="89" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>36</v>
       </c>
@@ -21474,7 +21474,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="90" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>28</v>
       </c>
@@ -21701,7 +21701,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="91" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>13</v>
       </c>
@@ -21928,7 +21928,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="92" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>52</v>
       </c>
@@ -22155,7 +22155,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="93" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>36</v>
       </c>
@@ -22382,7 +22382,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="94" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>13</v>
       </c>
@@ -22609,7 +22609,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="95" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>28</v>
       </c>
@@ -22836,7 +22836,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="96" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>28</v>
       </c>
@@ -23063,7 +23063,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="97" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>52</v>
       </c>
@@ -23290,7 +23290,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="98" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>36</v>
       </c>
@@ -23517,7 +23517,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="99" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>148</v>
       </c>
@@ -23744,7 +23744,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="100" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>28</v>
       </c>
@@ -23971,7 +23971,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="101" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>13</v>
       </c>
@@ -24198,7 +24198,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>36</v>
       </c>
@@ -24425,7 +24425,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>13</v>
       </c>
@@ -24652,7 +24652,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>32</v>
       </c>
@@ -24879,7 +24879,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="105" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>28</v>
       </c>
@@ -25106,7 +25106,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="106" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>28</v>
       </c>
@@ -25333,7 +25333,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="107" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>13</v>
       </c>
@@ -25560,7 +25560,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="108" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>32</v>
       </c>
@@ -25796,13 +25796,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ADD8185-3D8D-4FB6-A4B3-112D97C93F8A}">
   <dimension ref="A1:BX108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A1" t="str" cm="1">
         <f t="array" ref="A1:BX1">TRANSPOSE([1]Spalten_Ausw_Bez!H3:H78)</f>
         <v>PD_2</v>
@@ -26033,7 +26033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -26260,7 +26260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -26487,7 +26487,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -26714,7 +26714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -26941,7 +26941,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -27168,7 +27168,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -27395,7 +27395,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -27622,7 +27622,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -27849,7 +27849,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -28076,7 +28076,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -28303,7 +28303,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -28530,7 +28530,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -28757,7 +28757,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -28984,7 +28984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -29211,7 +29211,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -29438,7 +29438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -29665,7 +29665,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -29892,7 +29892,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -30119,7 +30119,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -30346,7 +30346,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -30573,7 +30573,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -30800,7 +30800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -31027,7 +31027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -31254,7 +31254,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -31481,7 +31481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -31708,7 +31708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -31935,7 +31935,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -32162,7 +32162,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -32389,7 +32389,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>148</v>
       </c>
@@ -32616,7 +32616,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="31" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -32843,7 +32843,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -33070,7 +33070,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -33297,7 +33297,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -33524,7 +33524,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -33751,7 +33751,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -33978,7 +33978,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="37" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -34205,7 +34205,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>13</v>
       </c>
@@ -34432,7 +34432,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -34659,7 +34659,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>28</v>
       </c>
@@ -34886,7 +34886,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -35113,7 +35113,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -35340,7 +35340,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>32</v>
       </c>
@@ -35567,7 +35567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>36</v>
       </c>
@@ -35794,7 +35794,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>36</v>
       </c>
@@ -36021,7 +36021,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>28</v>
       </c>
@@ -36248,7 +36248,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>36</v>
       </c>
@@ -36475,7 +36475,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>36</v>
       </c>
@@ -36702,7 +36702,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>28</v>
       </c>
@@ -36929,7 +36929,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>32</v>
       </c>
@@ -37156,7 +37156,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>13</v>
       </c>
@@ -37383,7 +37383,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>32</v>
       </c>
@@ -37610,7 +37610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>36</v>
       </c>
@@ -37837,7 +37837,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>36</v>
       </c>
@@ -38064,7 +38064,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>36</v>
       </c>
@@ -38291,7 +38291,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>13</v>
       </c>
@@ -38518,7 +38518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>28</v>
       </c>
@@ -38745,7 +38745,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>28</v>
       </c>
@@ -38972,7 +38972,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>28</v>
       </c>
@@ -39199,7 +39199,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>52</v>
       </c>
@@ -39426,7 +39426,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>32</v>
       </c>
@@ -39653,7 +39653,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>32</v>
       </c>
@@ -39880,7 +39880,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>13</v>
       </c>
@@ -40107,7 +40107,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>36</v>
       </c>
@@ -40334,7 +40334,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>36</v>
       </c>
@@ -40561,7 +40561,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>32</v>
       </c>
@@ -40788,7 +40788,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>13</v>
       </c>
@@ -41015,7 +41015,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>13</v>
       </c>
@@ -41242,7 +41242,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>36</v>
       </c>
@@ -41469,7 +41469,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>36</v>
       </c>
@@ -41696,7 +41696,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>13</v>
       </c>
@@ -41923,7 +41923,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>28</v>
       </c>
@@ -42150,7 +42150,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>52</v>
       </c>
@@ -42377,7 +42377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>52</v>
       </c>
@@ -42604,7 +42604,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>28</v>
       </c>
@@ -42831,7 +42831,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>28</v>
       </c>
@@ -43058,7 +43058,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>36</v>
       </c>
@@ -43285,7 +43285,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>28</v>
       </c>
@@ -43512,7 +43512,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>36</v>
       </c>
@@ -43739,7 +43739,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>28</v>
       </c>
@@ -43966,7 +43966,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>13</v>
       </c>
@@ -44193,7 +44193,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>36</v>
       </c>
@@ -44420,7 +44420,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>32</v>
       </c>
@@ -44647,7 +44647,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>28</v>
       </c>
@@ -44874,7 +44874,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>28</v>
       </c>
@@ -45101,7 +45101,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>28</v>
       </c>
@@ -45328,7 +45328,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>13</v>
       </c>
@@ -45555,7 +45555,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>13</v>
       </c>
@@ -45782,7 +45782,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>36</v>
       </c>
@@ -46009,7 +46009,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>28</v>
       </c>
@@ -46236,7 +46236,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>13</v>
       </c>
@@ -46463,7 +46463,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>52</v>
       </c>
@@ -46690,7 +46690,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>36</v>
       </c>
@@ -46917,7 +46917,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>13</v>
       </c>
@@ -47144,7 +47144,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>28</v>
       </c>
@@ -47371,7 +47371,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>28</v>
       </c>
@@ -47598,7 +47598,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>52</v>
       </c>
@@ -47825,7 +47825,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>36</v>
       </c>
@@ -48052,7 +48052,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>148</v>
       </c>
@@ -48279,7 +48279,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>28</v>
       </c>
@@ -48506,7 +48506,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>13</v>
       </c>
@@ -48733,7 +48733,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>36</v>
       </c>
@@ -48960,7 +48960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>13</v>
       </c>
@@ -49187,7 +49187,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>32</v>
       </c>
@@ -49414,7 +49414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>28</v>
       </c>
@@ -49641,7 +49641,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>28</v>
       </c>
@@ -49868,7 +49868,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>13</v>
       </c>
@@ -50095,7 +50095,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>32</v>
       </c>

</xml_diff>